<commit_message>
IDEFICS-1 corrected L44c to L44 and removed duplicate of J39a
</commit_message>
<xml_diff>
--- a/analyst/Franzi/rmonize/data_dictionary/DD_IDEFICS_FRANZI.xlsx
+++ b/analyst/Franzi/rmonize/data_dictionary/DD_IDEFICS_FRANZI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projekte\NFDI4Health\TA5\Pilotprojekte\Harmonisierung\HarmonizR\use-cases-harmonisation\analyst\Franzi\rmonize\data_dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{D8DCC441-9E70-40A4-8372-EC4174583D94}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{0D96819F-89DC-4142-ABC4-651404EFB6CD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="152">
   <si>
     <t>index</t>
   </si>
@@ -474,6 +474,9 @@
   </si>
   <si>
     <t>decimal</t>
+  </si>
+  <si>
+    <t>L44</t>
   </si>
 </sst>
 </file>
@@ -870,10 +873,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D75"/>
+  <dimension ref="A1:D74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="I71" sqref="I71"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A60" sqref="A60:XFD60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -974,7 +977,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>14</v>
+        <v>151</v>
       </c>
       <c r="C9" t="s">
         <v>19</v>
@@ -1535,10 +1538,10 @@
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C60" t="s">
-        <v>37</v>
+        <v>72</v>
       </c>
       <c r="D60" t="s">
         <v>150</v>
@@ -1546,10 +1549,10 @@
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C61" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D61" t="s">
         <v>150</v>
@@ -1557,10 +1560,10 @@
     </row>
     <row r="62" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C62" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D62" t="s">
         <v>150</v>
@@ -1568,10 +1571,10 @@
     </row>
     <row r="63" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C63" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D63" t="s">
         <v>150</v>
@@ -1579,10 +1582,10 @@
     </row>
     <row r="64" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C64" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D64" t="s">
         <v>150</v>
@@ -1590,10 +1593,10 @@
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C65" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D65" t="s">
         <v>150</v>
@@ -1601,10 +1604,10 @@
     </row>
     <row r="66" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C66" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D66" t="s">
         <v>150</v>
@@ -1612,10 +1615,10 @@
     </row>
     <row r="67" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C67" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D67" t="s">
         <v>150</v>
@@ -1623,10 +1626,10 @@
     </row>
     <row r="68" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C68" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D68" t="s">
         <v>150</v>
@@ -1634,10 +1637,10 @@
     </row>
     <row r="69" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C69" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D69" t="s">
         <v>150</v>
@@ -1645,10 +1648,10 @@
     </row>
     <row r="70" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C70" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D70" t="s">
         <v>150</v>
@@ -1656,10 +1659,10 @@
     </row>
     <row r="71" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C71" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D71" t="s">
         <v>150</v>
@@ -1667,10 +1670,10 @@
     </row>
     <row r="72" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C72" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D72" t="s">
         <v>150</v>
@@ -1678,10 +1681,10 @@
     </row>
     <row r="73" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C73" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D73" t="s">
         <v>150</v>
@@ -1689,23 +1692,12 @@
     </row>
     <row r="74" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C74" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D74" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="75" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B75" t="s">
-        <v>87</v>
-      </c>
-      <c r="C75" t="s">
-        <v>86</v>
-      </c>
-      <c r="D75" t="s">
         <v>150</v>
       </c>
     </row>

</xml_diff>

<commit_message>
IDEFICS-1 corrected DD and attached respective comparison file
</commit_message>
<xml_diff>
--- a/analyst/Franzi/rmonize/data_dictionary/DD_IDEFICS_FRANZI.xlsx
+++ b/analyst/Franzi/rmonize/data_dictionary/DD_IDEFICS_FRANZI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projekte\NFDI4Health\TA5\Pilotprojekte\Harmonisierung\HarmonizR\use-cases-harmonisation\analyst\Franzi\rmonize\data_dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{0D96819F-89DC-4142-ABC4-651404EFB6CD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{3AB76D18-2881-4562-982F-271645E34D67}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="154">
   <si>
     <t>index</t>
   </si>
@@ -477,6 +477,12 @@
   </si>
   <si>
     <t>L44</t>
+  </si>
+  <si>
+    <t>J38c</t>
+  </si>
+  <si>
+    <t>SACANA FGS J38c "Sweetened cheese and curd"</t>
   </si>
 </sst>
 </file>
@@ -873,10 +879,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D74"/>
+  <dimension ref="A1:D75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A60" sqref="A60:XFD60"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1164,10 +1170,10 @@
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>136</v>
+        <v>152</v>
       </c>
       <c r="C26" t="s">
-        <v>38</v>
+        <v>153</v>
       </c>
       <c r="D26" t="s">
         <v>150</v>
@@ -1175,10 +1181,10 @@
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C27" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D27" t="s">
         <v>150</v>
@@ -1186,10 +1192,10 @@
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C28" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D28" t="s">
         <v>150</v>
@@ -1197,10 +1203,10 @@
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C29" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D29" t="s">
         <v>150</v>
@@ -1208,10 +1214,10 @@
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C30" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D30" t="s">
         <v>150</v>
@@ -1219,10 +1225,10 @@
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C31" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D31" t="s">
         <v>150</v>
@@ -1230,10 +1236,10 @@
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C32" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D32" t="s">
         <v>150</v>
@@ -1241,10 +1247,10 @@
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C33" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D33" t="s">
         <v>150</v>
@@ -1252,10 +1258,10 @@
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C34" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D34" t="s">
         <v>150</v>
@@ -1263,10 +1269,10 @@
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C35" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D35" t="s">
         <v>150</v>
@@ -1274,10 +1280,10 @@
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C36" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D36" t="s">
         <v>150</v>
@@ -1285,10 +1291,10 @@
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C37" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D37" t="s">
         <v>150</v>
@@ -1296,10 +1302,10 @@
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C38" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D38" t="s">
         <v>150</v>
@@ -1307,10 +1313,10 @@
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C39" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D39" t="s">
         <v>150</v>
@@ -1318,10 +1324,10 @@
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C40" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D40" t="s">
         <v>150</v>
@@ -1329,10 +1335,10 @@
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C41" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D41" t="s">
         <v>150</v>
@@ -1340,10 +1346,10 @@
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C42" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D42" t="s">
         <v>150</v>
@@ -1351,10 +1357,10 @@
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C43" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D43" t="s">
         <v>150</v>
@@ -1362,10 +1368,10 @@
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C44" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D44" t="s">
         <v>150</v>
@@ -1373,10 +1379,10 @@
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C45" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D45" t="s">
         <v>150</v>
@@ -1384,10 +1390,10 @@
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C46" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D46" t="s">
         <v>150</v>
@@ -1395,10 +1401,10 @@
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C47" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D47" t="s">
         <v>150</v>
@@ -1406,10 +1412,10 @@
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C48" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D48" t="s">
         <v>150</v>
@@ -1417,10 +1423,10 @@
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C49" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D49" t="s">
         <v>150</v>
@@ -1428,10 +1434,10 @@
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C50" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D50" t="s">
         <v>150</v>
@@ -1439,10 +1445,10 @@
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C51" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D51" t="s">
         <v>150</v>
@@ -1450,10 +1456,10 @@
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C52" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D52" t="s">
         <v>150</v>
@@ -1461,10 +1467,10 @@
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C53" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D53" t="s">
         <v>150</v>
@@ -1472,10 +1478,10 @@
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C54" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D54" t="s">
         <v>150</v>
@@ -1483,10 +1489,10 @@
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C55" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D55" t="s">
         <v>150</v>
@@ -1494,10 +1500,10 @@
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C56" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D56" t="s">
         <v>150</v>
@@ -1505,10 +1511,10 @@
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C57" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D57" t="s">
         <v>150</v>
@@ -1516,10 +1522,10 @@
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C58" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D58" t="s">
         <v>150</v>
@@ -1527,10 +1533,10 @@
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C59" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D59" t="s">
         <v>150</v>
@@ -1538,10 +1544,10 @@
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C60" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D60" t="s">
         <v>150</v>
@@ -1549,10 +1555,10 @@
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C61" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D61" t="s">
         <v>150</v>
@@ -1560,10 +1566,10 @@
     </row>
     <row r="62" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C62" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D62" t="s">
         <v>150</v>
@@ -1571,10 +1577,10 @@
     </row>
     <row r="63" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C63" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D63" t="s">
         <v>150</v>
@@ -1582,10 +1588,10 @@
     </row>
     <row r="64" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C64" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D64" t="s">
         <v>150</v>
@@ -1593,10 +1599,10 @@
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C65" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D65" t="s">
         <v>150</v>
@@ -1604,10 +1610,10 @@
     </row>
     <row r="66" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C66" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D66" t="s">
         <v>150</v>
@@ -1615,10 +1621,10 @@
     </row>
     <row r="67" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C67" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D67" t="s">
         <v>150</v>
@@ -1626,10 +1632,10 @@
     </row>
     <row r="68" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C68" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D68" t="s">
         <v>150</v>
@@ -1637,10 +1643,10 @@
     </row>
     <row r="69" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C69" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D69" t="s">
         <v>150</v>
@@ -1648,10 +1654,10 @@
     </row>
     <row r="70" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C70" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D70" t="s">
         <v>150</v>
@@ -1659,10 +1665,10 @@
     </row>
     <row r="71" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C71" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D71" t="s">
         <v>150</v>
@@ -1670,10 +1676,10 @@
     </row>
     <row r="72" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C72" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D72" t="s">
         <v>150</v>
@@ -1681,10 +1687,10 @@
     </row>
     <row r="73" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C73" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D73" t="s">
         <v>150</v>
@@ -1692,12 +1698,23 @@
     </row>
     <row r="74" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
+        <v>88</v>
+      </c>
+      <c r="C74" t="s">
+        <v>85</v>
+      </c>
+      <c r="D74" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="75" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B75" t="s">
         <v>87</v>
       </c>
-      <c r="C74" t="s">
+      <c r="C75" t="s">
         <v>86</v>
       </c>
-      <c r="D74" t="s">
+      <c r="D75" t="s">
         <v>150</v>
       </c>
     </row>

</xml_diff>